<commit_message>
make it so that loads total number of questions by reading the dom
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="10260" yWindow="120" windowWidth="39600" windowHeight="26020" tabRatio="500"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <si>
     <t>question</t>
   </si>
@@ -245,24 +245,6 @@
     <t>Brown outs sometimes occur when there is a heavy load on the grid. New technologies that improve reliability are helping to prevent brown outs and blackouts.</t>
   </si>
   <si>
-    <t>Who is involved in making sure the grid stays up and running?</t>
-  </si>
-  <si>
-    <t>All of the above</t>
-  </si>
-  <si>
-    <t>Utility companies</t>
-  </si>
-  <si>
-    <t>State and local government</t>
-  </si>
-  <si>
-    <t>The federal government</t>
-  </si>
-  <si>
-    <t>The electrical grid is a complicated network that relies on private and public partners working together to make sure the power keeps flowing.</t>
-  </si>
-  <si>
     <t>http://energy.gov/sites/prod/files/image1grid.jpg</t>
   </si>
   <si>
@@ -291,9 +273,6 @@
   </si>
   <si>
     <t>http://energy.gov/sites/prod/files/image10grid.jpg</t>
-  </si>
-  <si>
-    <t>http://energy.gov/sites/prod/files/image11grid.jpg</t>
   </si>
   <si>
     <t>Part of a television antenna</t>
@@ -715,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -753,7 +732,7 @@
     </row>
     <row r="2" spans="1:7" ht="60">
       <c r="A2" s="3" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>18</v>
@@ -765,10 +744,10 @@
         <v>20</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>21</v>
@@ -776,7 +755,7 @@
     </row>
     <row r="3" spans="1:7" ht="30">
       <c r="A3" s="3" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>22</v>
@@ -791,7 +770,7 @@
         <v>25</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>26</v>
@@ -814,7 +793,7 @@
         <v>31</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>32</v>
@@ -834,10 +813,10 @@
         <v>36</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>37</v>
@@ -860,7 +839,7 @@
         <v>42</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>43</v>
@@ -883,7 +862,7 @@
         <v>48</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>49</v>
@@ -906,7 +885,7 @@
         <v>54</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>55</v>
@@ -929,7 +908,7 @@
         <v>60</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>61</v>
@@ -952,7 +931,7 @@
         <v>66</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>67</v>
@@ -975,33 +954,10 @@
         <v>72</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="30">
-      <c r="A12" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1039,7 +995,7 @@
     </row>
     <row r="2" spans="1:2" ht="30">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>11</v>

</xml_diff>